<commit_message>
Validar data no serializer e troca do modelo xgboost pelo Rf regressor
</commit_message>
<xml_diff>
--- a/modelosML/Consumos/consumo_agua.xlsx
+++ b/modelosML/Consumos/consumo_agua.xlsx
@@ -1798,7 +1798,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="54">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1958,9 +1958,6 @@
     </xf>
     <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2275,8 +2272,8 @@
     <col min="3" max="3" style="51" width="14.576428571428572" customWidth="1" bestFit="1"/>
     <col min="4" max="4" style="52" width="21.719285714285714" customWidth="1" bestFit="1"/>
     <col min="5" max="5" style="53" width="26.14785714285714" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="54" width="10.290714285714287" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="54" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="50" width="10.290714285714287" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="50" width="13.576428571428572" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="29.25" customFormat="1" s="1">

</xml_diff>